<commit_message>
Lexicon code is functional
Need to add debugging tools/error throwing for when files/allophones can't be found and make everything a bit more user friendly, but it works!  I'll probably add a few more corrections because some of the allophones don't translate very well.
</commit_message>
<xml_diff>
--- a/documentation/speechsynth.xlsx
+++ b/documentation/speechsynth.xlsx
@@ -1813,7 +1813,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1823,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>